<commit_message>
Fixed to work with Ximena
</commit_message>
<xml_diff>
--- a/worklist.xlsx
+++ b/worklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabewilson/Desktop/worklist_generation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3241FD07-51B1-D843-BB14-40E3C738CAEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513F84CB-3474-D645-AF45-B06392CE0D95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="740" windowWidth="29400" windowHeight="17100" xr2:uid="{BF50EA0A-2797-EC49-8565-645DB7B38C61}"/>
+    <workbookView xWindow="-20" yWindow="740" windowWidth="29400" windowHeight="17080" xr2:uid="{BF50EA0A-2797-EC49-8565-645DB7B38C61}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,9 +41,6 @@
     <t>Notebook code:</t>
   </si>
   <si>
-    <t>GW0711</t>
-  </si>
-  <si>
     <t>Number:</t>
   </si>
   <si>
@@ -257,9 +254,6 @@
     <t>digest_mix</t>
   </si>
   <si>
-    <t>1 column</t>
-  </si>
-  <si>
     <t>Experiment One</t>
   </si>
   <si>
@@ -330,6 +324,12 @@
   </si>
   <si>
     <t>1-30</t>
+  </si>
+  <si>
+    <t>2 column</t>
+  </si>
+  <si>
+    <t>GW0821</t>
   </si>
 </sst>
 </file>
@@ -358,7 +358,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -373,7 +373,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -559,7 +571,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
@@ -642,13 +654,66 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -985,9 +1050,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79332BF3-487A-D048-AE38-CBE359952258}">
   <dimension ref="A1:AS58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="40" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AD28" sqref="AD28"/>
+      <selection pane="bottomLeft" activeCell="AE20" sqref="AE20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1018,102 +1083,102 @@
         <v>0</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>1</v>
+        <v>97</v>
       </c>
       <c r="AD1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="AE1" s="14" t="s">
+      <c r="AF1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="AF1" s="35" t="s">
+      <c r="AG1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="AG1" s="11" t="s">
+      <c r="AH1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="AH1" s="14" t="s">
+      <c r="AI1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="AI1" s="16" t="s">
+      <c r="AJ1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="AJ1" s="15" t="s">
+      <c r="AK1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="AK1" s="14" t="s">
+      <c r="AL1" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="AL1" s="35" t="s">
+      <c r="AM1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="AM1" s="11" t="s">
+      <c r="AN1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="AN1" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO1" s="37" t="s">
+      <c r="AO1" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP1" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="AP1" s="14" t="s">
-        <v>61</v>
-      </c>
       <c r="AQ1" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AR1" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="AS1" s="17" t="s">
         <v>93</v>
-      </c>
-      <c r="AR1" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="AS1" s="17" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="AD2" s="54">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF2" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG2" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="AD2" s="11">
-        <v>1</v>
-      </c>
-      <c r="AE2" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="AF2" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="AG2" s="5" t="s">
+      <c r="AH2" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="AH2" s="18" t="s">
+      <c r="AI2" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="AJ2" s="49" t="s">
+        <v>17</v>
+      </c>
+      <c r="AK2" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL2" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="AM2" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="AI2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="AJ2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="AK2" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="AL2" s="34" t="s">
+      <c r="AN2" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="AM2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AN2" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="AO2" s="38">
-        <v>1</v>
-      </c>
-      <c r="AP2" s="21" t="s">
-        <v>62</v>
+      <c r="AO2" s="51">
+        <v>1</v>
+      </c>
+      <c r="AP2" s="52" t="s">
+        <v>61</v>
       </c>
       <c r="AQ2" s="21"/>
       <c r="AR2" s="21"/>
@@ -1121,49 +1186,49 @@
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="AD3" s="12">
         <v>2</v>
       </c>
       <c r="AE3" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AF3" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AG3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="AH3" s="18" t="s">
+      <c r="AI3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="AJ3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AK3" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL3" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="AM3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="AI3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="AJ3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="AK3" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="AL3" s="34" t="s">
+      <c r="AN3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="AM3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AN3" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="AO3" s="39">
+      <c r="AO3" s="37">
         <v>1</v>
       </c>
       <c r="AP3" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AQ3" s="21">
         <v>10</v>
@@ -1207,40 +1272,40 @@
         <v>3</v>
       </c>
       <c r="AE4" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF4" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="AF4" s="34" t="s">
-        <v>72</v>
-      </c>
       <c r="AG4" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="AH4" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="AJ4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AK4" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL4" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="AM4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="AI4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="AJ4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="AK4" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="AL4" s="34" t="s">
+      <c r="AN4" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="AM4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AN4" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="AO4" s="39">
+      <c r="AO4" s="37">
         <v>1</v>
       </c>
       <c r="AP4" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AQ4" s="21">
         <v>10</v>
@@ -1254,13 +1319,13 @@
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="D5" t="s">
         <v>25</v>
-      </c>
-      <c r="D5" t="s">
-        <v>26</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -1334,44 +1399,44 @@
       <c r="AB5">
         <v>24</v>
       </c>
-      <c r="AD5" s="12">
+      <c r="AD5" s="55">
         <v>4</v>
       </c>
-      <c r="AE5" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="AF5" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="AG5" s="5" t="s">
+      <c r="AE5" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF5" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG5" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH5" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="AH5" s="18" t="s">
+      <c r="AI5" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AJ5" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="AK5" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL5" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="AM5" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="AI5" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="AJ5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="AK5" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="AL5" s="34" t="s">
+      <c r="AN5" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="AM5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AN5" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="AO5" s="39">
+      <c r="AO5" s="53">
         <v>2</v>
       </c>
-      <c r="AP5" s="21" t="s">
-        <v>62</v>
+      <c r="AP5" s="44" t="s">
+        <v>61</v>
       </c>
       <c r="AQ5" s="21"/>
       <c r="AR5" s="21"/>
@@ -1379,13 +1444,13 @@
     </row>
     <row r="6" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="D6" t="s">
         <v>28</v>
-      </c>
-      <c r="D6" t="s">
-        <v>29</v>
       </c>
       <c r="E6" s="2">
         <v>30</v>
@@ -1413,44 +1478,44 @@
       <c r="Z6" s="3"/>
       <c r="AA6" s="3"/>
       <c r="AB6" s="4"/>
-      <c r="AD6" s="12">
+      <c r="AD6" s="56">
         <v>5</v>
       </c>
-      <c r="AE6" s="18" t="s">
+      <c r="AE6" s="57" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF6" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="AF6" s="34" t="s">
-        <v>80</v>
-      </c>
-      <c r="AG6" s="5" t="s">
+      <c r="AG6" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH6" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="AH6" s="18" t="s">
+      <c r="AI6" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="AJ6" s="61" t="s">
+        <v>17</v>
+      </c>
+      <c r="AK6" s="57" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL6" s="58" t="s">
+        <v>19</v>
+      </c>
+      <c r="AM6" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="AI6" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="AJ6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="AK6" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="AL6" s="34" t="s">
+      <c r="AN6" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="AM6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AN6" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="AO6" s="39">
-        <v>1</v>
-      </c>
-      <c r="AP6" s="21" t="s">
-        <v>62</v>
+      <c r="AO6" s="62">
+        <v>1</v>
+      </c>
+      <c r="AP6" s="63" t="s">
+        <v>61</v>
       </c>
       <c r="AQ6" s="21"/>
       <c r="AR6" s="21"/>
@@ -1458,7 +1523,7 @@
     </row>
     <row r="7" spans="1:45" x14ac:dyDescent="0.2">
       <c r="D7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="6"/>
@@ -1497,7 +1562,7 @@
       <c r="AL7" s="34"/>
       <c r="AM7" s="5"/>
       <c r="AN7" s="18"/>
-      <c r="AO7" s="39"/>
+      <c r="AO7" s="37"/>
       <c r="AP7" s="21"/>
       <c r="AQ7" s="21"/>
       <c r="AR7" s="21"/>
@@ -1505,68 +1570,68 @@
     </row>
     <row r="8" spans="1:45" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="6"/>
-      <c r="G8" s="6">
-        <v>1</v>
-      </c>
-      <c r="H8" s="6">
-        <v>1</v>
-      </c>
-      <c r="I8" s="6">
-        <v>1</v>
-      </c>
-      <c r="J8" s="6">
-        <v>1</v>
-      </c>
-      <c r="K8" s="6">
-        <v>1</v>
-      </c>
-      <c r="L8" s="6">
-        <v>1</v>
-      </c>
-      <c r="M8" s="6">
-        <v>1</v>
-      </c>
-      <c r="N8" s="6">
-        <v>1</v>
-      </c>
-      <c r="O8" s="6">
-        <v>1</v>
-      </c>
-      <c r="P8" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="6">
-        <v>1</v>
-      </c>
-      <c r="R8" s="6">
-        <v>1</v>
-      </c>
-      <c r="S8" s="6">
-        <v>1</v>
-      </c>
-      <c r="T8" s="6">
-        <v>1</v>
-      </c>
-      <c r="U8" s="6">
-        <v>1</v>
-      </c>
-      <c r="V8" s="6">
-        <v>1</v>
-      </c>
-      <c r="W8" s="6">
-        <v>1</v>
-      </c>
-      <c r="X8" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y8" s="6">
-        <v>1</v>
-      </c>
-      <c r="Z8" s="6">
+      <c r="G8" s="49">
+        <v>1</v>
+      </c>
+      <c r="H8" s="49">
+        <v>1</v>
+      </c>
+      <c r="I8" s="49">
+        <v>1</v>
+      </c>
+      <c r="J8" s="49">
+        <v>1</v>
+      </c>
+      <c r="K8" s="49">
+        <v>1</v>
+      </c>
+      <c r="L8" s="49">
+        <v>1</v>
+      </c>
+      <c r="M8" s="49">
+        <v>1</v>
+      </c>
+      <c r="N8" s="49">
+        <v>1</v>
+      </c>
+      <c r="O8" s="49">
+        <v>1</v>
+      </c>
+      <c r="P8" s="49">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="49">
+        <v>1</v>
+      </c>
+      <c r="R8" s="49">
+        <v>1</v>
+      </c>
+      <c r="S8" s="49">
+        <v>1</v>
+      </c>
+      <c r="T8" s="49">
+        <v>1</v>
+      </c>
+      <c r="U8" s="49">
+        <v>1</v>
+      </c>
+      <c r="V8" s="49">
+        <v>1</v>
+      </c>
+      <c r="W8" s="49">
+        <v>1</v>
+      </c>
+      <c r="X8" s="49">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="49">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="49">
         <v>1</v>
       </c>
       <c r="AA8" s="6"/>
@@ -1575,40 +1640,40 @@
         <v>7</v>
       </c>
       <c r="AE8" s="18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="AF8" s="34" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="AG8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH8" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="AH8" s="18" t="s">
+      <c r="AI8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="AJ8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AK8" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL8" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="AM8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="AI8" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="AJ8" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="AK8" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="AL8" s="34" t="s">
+      <c r="AN8" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="AM8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AN8" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="AO8" s="39">
+      <c r="AO8" s="37">
         <v>1</v>
       </c>
       <c r="AP8" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AQ8" s="21"/>
       <c r="AR8" s="21"/>
@@ -1616,7 +1681,7 @@
     </row>
     <row r="9" spans="1:45" x14ac:dyDescent="0.2">
       <c r="D9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="6"/>
@@ -1686,40 +1751,40 @@
         <v>8</v>
       </c>
       <c r="AE9" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF9" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="AF9" s="34" t="s">
-        <v>70</v>
-      </c>
       <c r="AG9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH9" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="AH9" s="18" t="s">
+      <c r="AI9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="AJ9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AK9" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL9" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="AM9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="AI9" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="AJ9" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="AK9" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="AL9" s="34" t="s">
+      <c r="AN9" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="AM9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AN9" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="AO9" s="39">
+      <c r="AO9" s="37">
         <v>1</v>
       </c>
       <c r="AP9" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AQ9" s="21"/>
       <c r="AR9" s="21"/>
@@ -1727,7 +1792,7 @@
     </row>
     <row r="10" spans="1:45" x14ac:dyDescent="0.2">
       <c r="D10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="6"/>
@@ -1797,40 +1862,40 @@
         <v>9</v>
       </c>
       <c r="AE10" s="18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="AF10" s="34" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="AG10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH10" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="AH10" s="18" t="s">
+      <c r="AI10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="AJ10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AK10" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL10" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="AM10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="AI10" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="AJ10" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="AK10" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="AL10" s="34" t="s">
+      <c r="AN10" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="AM10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AN10" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="AO10" s="39">
+      <c r="AO10" s="37">
         <v>1</v>
       </c>
       <c r="AP10" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AQ10" s="21"/>
       <c r="AR10" s="21"/>
@@ -1838,80 +1903,110 @@
     </row>
     <row r="11" spans="1:45" x14ac:dyDescent="0.2">
       <c r="D11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="6"/>
-      <c r="G11" s="6">
+      <c r="G11" s="42">
         <v>4</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="42">
         <v>4</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="42">
         <v>4</v>
       </c>
-      <c r="J11" s="6">
+      <c r="J11" s="42">
         <v>4</v>
       </c>
-      <c r="K11" s="6">
+      <c r="K11" s="42">
         <v>4</v>
       </c>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
-      <c r="S11" s="6"/>
-      <c r="T11" s="6"/>
-      <c r="U11" s="6"/>
-      <c r="V11" s="6"/>
-      <c r="W11" s="6"/>
-      <c r="X11" s="6"/>
-      <c r="Y11" s="6"/>
-      <c r="Z11" s="6"/>
+      <c r="L11" s="42">
+        <v>4</v>
+      </c>
+      <c r="M11" s="42">
+        <v>4</v>
+      </c>
+      <c r="N11" s="42">
+        <v>4</v>
+      </c>
+      <c r="O11" s="42">
+        <v>4</v>
+      </c>
+      <c r="P11" s="42">
+        <v>4</v>
+      </c>
+      <c r="Q11" s="42">
+        <v>4</v>
+      </c>
+      <c r="R11" s="42">
+        <v>4</v>
+      </c>
+      <c r="S11" s="42">
+        <v>4</v>
+      </c>
+      <c r="T11" s="42">
+        <v>4</v>
+      </c>
+      <c r="U11" s="42">
+        <v>4</v>
+      </c>
+      <c r="V11" s="42">
+        <v>4</v>
+      </c>
+      <c r="W11" s="42">
+        <v>4</v>
+      </c>
+      <c r="X11" s="42">
+        <v>4</v>
+      </c>
+      <c r="Y11" s="42">
+        <v>4</v>
+      </c>
+      <c r="Z11" s="42">
+        <v>4</v>
+      </c>
       <c r="AA11" s="6"/>
       <c r="AB11" s="7"/>
       <c r="AD11" s="12">
         <v>10</v>
       </c>
       <c r="AE11" s="18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="AF11" s="34" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="AG11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH11" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="AH11" s="18" t="s">
+      <c r="AI11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="AJ11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AK11" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL11" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="AM11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="AI11" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="AJ11" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="AK11" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="AL11" s="34" t="s">
+      <c r="AN11" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="AM11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AN11" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="AO11" s="39">
+      <c r="AO11" s="37">
         <v>1</v>
       </c>
       <c r="AP11" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AQ11" s="21"/>
       <c r="AR11" s="21"/>
@@ -1919,68 +2014,68 @@
     </row>
     <row r="12" spans="1:45" x14ac:dyDescent="0.2">
       <c r="D12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="6">
+      <c r="G12" s="61">
         <v>5</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="61">
         <v>5</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="61">
         <v>5</v>
       </c>
-      <c r="J12" s="6">
+      <c r="J12" s="61">
         <v>5</v>
       </c>
-      <c r="K12" s="6">
+      <c r="K12" s="61">
         <v>5</v>
       </c>
-      <c r="L12" s="6">
+      <c r="L12" s="61">
         <v>5</v>
       </c>
-      <c r="M12" s="6">
+      <c r="M12" s="61">
         <v>5</v>
       </c>
-      <c r="N12" s="6">
+      <c r="N12" s="61">
         <v>5</v>
       </c>
-      <c r="O12" s="6">
+      <c r="O12" s="61">
         <v>5</v>
       </c>
-      <c r="P12" s="6">
+      <c r="P12" s="61">
         <v>5</v>
       </c>
-      <c r="Q12" s="6">
+      <c r="Q12" s="61">
         <v>5</v>
       </c>
-      <c r="R12" s="6">
+      <c r="R12" s="61">
         <v>5</v>
       </c>
-      <c r="S12" s="6">
+      <c r="S12" s="61">
         <v>5</v>
       </c>
-      <c r="T12" s="6">
+      <c r="T12" s="61">
         <v>5</v>
       </c>
-      <c r="U12" s="6">
+      <c r="U12" s="61">
         <v>5</v>
       </c>
-      <c r="V12" s="6">
+      <c r="V12" s="61">
         <v>5</v>
       </c>
-      <c r="W12" s="6">
+      <c r="W12" s="61">
         <v>5</v>
       </c>
-      <c r="X12" s="6">
+      <c r="X12" s="61">
         <v>5</v>
       </c>
-      <c r="Y12" s="6">
+      <c r="Y12" s="61">
         <v>5</v>
       </c>
-      <c r="Z12" s="6">
+      <c r="Z12" s="61">
         <v>5</v>
       </c>
       <c r="AA12" s="6"/>
@@ -1989,40 +2084,40 @@
         <v>11</v>
       </c>
       <c r="AE12" s="18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AF12" s="34" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="AG12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH12" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="AH12" s="18" t="s">
+      <c r="AI12" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="AJ12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AK12" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL12" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="AM12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="AI12" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="AJ12" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="AK12" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="AL12" s="34" t="s">
+      <c r="AN12" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="AM12" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AN12" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="AO12" s="39">
+      <c r="AO12" s="37">
         <v>1</v>
       </c>
       <c r="AP12" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AQ12" s="21"/>
       <c r="AR12" s="21"/>
@@ -2030,7 +2125,7 @@
     </row>
     <row r="13" spans="1:45" x14ac:dyDescent="0.2">
       <c r="D13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="6"/>
@@ -2060,40 +2155,40 @@
         <v>12</v>
       </c>
       <c r="AE13" s="18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AF13" s="34" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AG13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH13" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="AH13" s="18" t="s">
+      <c r="AI13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="AJ13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AK13" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL13" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="AM13" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="AI13" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="AJ13" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="AK13" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="AL13" s="34" t="s">
+      <c r="AN13" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="AM13" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AN13" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="AO13" s="39">
+      <c r="AO13" s="37">
         <v>1</v>
       </c>
       <c r="AP13" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AQ13" s="21"/>
       <c r="AR13" s="21"/>
@@ -2101,7 +2196,7 @@
     </row>
     <row r="14" spans="1:45" x14ac:dyDescent="0.2">
       <c r="D14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="6"/>
@@ -2140,7 +2235,7 @@
       <c r="AL14" s="34"/>
       <c r="AM14" s="5"/>
       <c r="AN14" s="18"/>
-      <c r="AO14" s="39"/>
+      <c r="AO14" s="37"/>
       <c r="AP14" s="21"/>
       <c r="AQ14" s="21"/>
       <c r="AR14" s="21"/>
@@ -2148,7 +2243,7 @@
     </row>
     <row r="15" spans="1:45" x14ac:dyDescent="0.2">
       <c r="D15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="6"/>
@@ -2187,7 +2282,7 @@
       <c r="AL15" s="34"/>
       <c r="AM15" s="5"/>
       <c r="AN15" s="18"/>
-      <c r="AO15" s="39"/>
+      <c r="AO15" s="37"/>
       <c r="AP15" s="21"/>
       <c r="AQ15" s="21"/>
       <c r="AR15" s="21"/>
@@ -2195,7 +2290,7 @@
     </row>
     <row r="16" spans="1:45" x14ac:dyDescent="0.2">
       <c r="D16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="6"/>
@@ -2238,7 +2333,7 @@
       <c r="AL16" s="34"/>
       <c r="AM16" s="5"/>
       <c r="AN16" s="18"/>
-      <c r="AO16" s="39"/>
+      <c r="AO16" s="37"/>
       <c r="AP16" s="21"/>
       <c r="AQ16" s="21"/>
       <c r="AR16" s="21"/>
@@ -2246,7 +2341,7 @@
     </row>
     <row r="17" spans="1:45" x14ac:dyDescent="0.2">
       <c r="D17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="6"/>
@@ -2285,7 +2380,7 @@
       <c r="AL17" s="34"/>
       <c r="AM17" s="5"/>
       <c r="AN17" s="18"/>
-      <c r="AO17" s="39"/>
+      <c r="AO17" s="37"/>
       <c r="AP17" s="21"/>
       <c r="AQ17" s="21"/>
       <c r="AR17" s="21"/>
@@ -2293,7 +2388,7 @@
     </row>
     <row r="18" spans="1:45" x14ac:dyDescent="0.2">
       <c r="D18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="6"/>
@@ -2332,7 +2427,7 @@
       <c r="AL18" s="34"/>
       <c r="AM18" s="5"/>
       <c r="AN18" s="18"/>
-      <c r="AO18" s="39"/>
+      <c r="AO18" s="37"/>
       <c r="AP18" s="21"/>
       <c r="AQ18" s="21"/>
       <c r="AR18" s="21"/>
@@ -2340,7 +2435,7 @@
     </row>
     <row r="19" spans="1:45" x14ac:dyDescent="0.2">
       <c r="D19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="6"/>
@@ -2379,7 +2474,7 @@
       <c r="AL19" s="34"/>
       <c r="AM19" s="5"/>
       <c r="AN19" s="18"/>
-      <c r="AO19" s="39"/>
+      <c r="AO19" s="37"/>
       <c r="AP19" s="21"/>
       <c r="AQ19" s="21"/>
       <c r="AR19" s="21"/>
@@ -2387,7 +2482,7 @@
     </row>
     <row r="20" spans="1:45" x14ac:dyDescent="0.2">
       <c r="D20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="6"/>
@@ -2426,7 +2521,7 @@
       <c r="AL20" s="34"/>
       <c r="AM20" s="5"/>
       <c r="AN20" s="18"/>
-      <c r="AO20" s="39"/>
+      <c r="AO20" s="37"/>
       <c r="AP20" s="21"/>
       <c r="AQ20" s="21"/>
       <c r="AR20" s="21"/>
@@ -2434,7 +2529,7 @@
     </row>
     <row r="21" spans="1:45" x14ac:dyDescent="0.2">
       <c r="D21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="9"/>
@@ -2473,7 +2568,7 @@
       <c r="AL21" s="34"/>
       <c r="AM21" s="5"/>
       <c r="AN21" s="18"/>
-      <c r="AO21" s="39"/>
+      <c r="AO21" s="37"/>
       <c r="AP21" s="21"/>
       <c r="AQ21" s="21"/>
       <c r="AR21" s="21"/>
@@ -2520,7 +2615,7 @@
       <c r="AL22" s="34"/>
       <c r="AM22" s="5"/>
       <c r="AN22" s="18"/>
-      <c r="AO22" s="39"/>
+      <c r="AO22" s="37"/>
       <c r="AP22" s="21"/>
       <c r="AQ22" s="21"/>
       <c r="AR22" s="21"/>
@@ -2528,13 +2623,13 @@
     </row>
     <row r="23" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="14" t="s">
-        <v>25</v>
-      </c>
       <c r="D23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -2621,7 +2716,7 @@
       <c r="AL23" s="34"/>
       <c r="AM23" s="5"/>
       <c r="AN23" s="18"/>
-      <c r="AO23" s="39"/>
+      <c r="AO23" s="37"/>
       <c r="AP23" s="21"/>
       <c r="AQ23" s="21"/>
       <c r="AR23" s="21"/>
@@ -2629,13 +2724,13 @@
     </row>
     <row r="24" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A24" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="3"/>
@@ -2674,7 +2769,7 @@
       <c r="AL24" s="34"/>
       <c r="AM24" s="5"/>
       <c r="AN24" s="18"/>
-      <c r="AO24" s="39"/>
+      <c r="AO24" s="37"/>
       <c r="AP24" s="21"/>
       <c r="AQ24" s="21"/>
       <c r="AR24" s="21"/>
@@ -2682,7 +2777,7 @@
     </row>
     <row r="25" spans="1:45" x14ac:dyDescent="0.2">
       <c r="D25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="6"/>
@@ -2721,7 +2816,7 @@
       <c r="AL25" s="34"/>
       <c r="AM25" s="5"/>
       <c r="AN25" s="18"/>
-      <c r="AO25" s="39"/>
+      <c r="AO25" s="37"/>
       <c r="AP25" s="21"/>
       <c r="AQ25" s="21"/>
       <c r="AR25" s="21"/>
@@ -2729,68 +2824,68 @@
     </row>
     <row r="26" spans="1:45" x14ac:dyDescent="0.2">
       <c r="D26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="6"/>
-      <c r="G26" s="6">
-        <v>1</v>
-      </c>
-      <c r="H26" s="6">
-        <v>1</v>
-      </c>
-      <c r="I26" s="6">
-        <v>1</v>
-      </c>
-      <c r="J26" s="6">
-        <v>1</v>
-      </c>
-      <c r="K26" s="6">
-        <v>1</v>
-      </c>
-      <c r="L26" s="6">
-        <v>1</v>
-      </c>
-      <c r="M26" s="6">
-        <v>1</v>
-      </c>
-      <c r="N26" s="6">
-        <v>1</v>
-      </c>
-      <c r="O26" s="6">
-        <v>1</v>
-      </c>
-      <c r="P26" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q26" s="6">
-        <v>1</v>
-      </c>
-      <c r="R26" s="6">
-        <v>1</v>
-      </c>
-      <c r="S26" s="6">
-        <v>1</v>
-      </c>
-      <c r="T26" s="6">
-        <v>1</v>
-      </c>
-      <c r="U26" s="6">
-        <v>1</v>
-      </c>
-      <c r="V26" s="6">
-        <v>1</v>
-      </c>
-      <c r="W26" s="6">
-        <v>1</v>
-      </c>
-      <c r="X26" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y26" s="6">
-        <v>1</v>
-      </c>
-      <c r="Z26" s="6">
+      <c r="G26" s="49">
+        <v>1</v>
+      </c>
+      <c r="H26" s="49">
+        <v>1</v>
+      </c>
+      <c r="I26" s="49">
+        <v>1</v>
+      </c>
+      <c r="J26" s="49">
+        <v>1</v>
+      </c>
+      <c r="K26" s="49">
+        <v>1</v>
+      </c>
+      <c r="L26" s="49">
+        <v>1</v>
+      </c>
+      <c r="M26" s="49">
+        <v>1</v>
+      </c>
+      <c r="N26" s="49">
+        <v>1</v>
+      </c>
+      <c r="O26" s="49">
+        <v>1</v>
+      </c>
+      <c r="P26" s="49">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="49">
+        <v>1</v>
+      </c>
+      <c r="R26" s="49">
+        <v>1</v>
+      </c>
+      <c r="S26" s="49">
+        <v>1</v>
+      </c>
+      <c r="T26" s="49">
+        <v>1</v>
+      </c>
+      <c r="U26" s="49">
+        <v>1</v>
+      </c>
+      <c r="V26" s="49">
+        <v>1</v>
+      </c>
+      <c r="W26" s="49">
+        <v>1</v>
+      </c>
+      <c r="X26" s="49">
+        <v>1</v>
+      </c>
+      <c r="Y26" s="49">
+        <v>1</v>
+      </c>
+      <c r="Z26" s="49">
         <v>1</v>
       </c>
       <c r="AA26" s="6"/>
@@ -2808,7 +2903,7 @@
       <c r="AL26" s="34"/>
       <c r="AM26" s="5"/>
       <c r="AN26" s="18"/>
-      <c r="AO26" s="39"/>
+      <c r="AO26" s="37"/>
       <c r="AP26" s="21"/>
       <c r="AQ26" s="21"/>
       <c r="AR26" s="21"/>
@@ -2816,7 +2911,7 @@
     </row>
     <row r="27" spans="1:45" x14ac:dyDescent="0.2">
       <c r="D27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="6"/>
@@ -2895,7 +2990,7 @@
       <c r="AL27" s="34"/>
       <c r="AM27" s="5"/>
       <c r="AN27" s="18"/>
-      <c r="AO27" s="39"/>
+      <c r="AO27" s="37"/>
       <c r="AP27" s="21"/>
       <c r="AQ27" s="21"/>
       <c r="AR27" s="21"/>
@@ -2903,7 +2998,7 @@
     </row>
     <row r="28" spans="1:45" x14ac:dyDescent="0.2">
       <c r="D28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="6"/>
@@ -2982,7 +3077,7 @@
       <c r="AL28" s="34"/>
       <c r="AM28" s="5"/>
       <c r="AN28" s="18"/>
-      <c r="AO28" s="39"/>
+      <c r="AO28" s="37"/>
       <c r="AP28" s="21"/>
       <c r="AQ28" s="21"/>
       <c r="AR28" s="21"/>
@@ -2990,30 +3085,70 @@
     </row>
     <row r="29" spans="1:45" x14ac:dyDescent="0.2">
       <c r="D29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
-      <c r="M29" s="6"/>
-      <c r="N29" s="6"/>
-      <c r="O29" s="6"/>
-      <c r="P29" s="6"/>
-      <c r="Q29" s="6"/>
-      <c r="R29" s="6"/>
-      <c r="S29" s="6"/>
-      <c r="T29" s="6"/>
-      <c r="U29" s="6"/>
-      <c r="V29" s="6"/>
-      <c r="W29" s="6"/>
-      <c r="X29" s="6"/>
-      <c r="Y29" s="6"/>
-      <c r="Z29" s="6"/>
+      <c r="G29" s="42">
+        <v>4</v>
+      </c>
+      <c r="H29" s="42">
+        <v>4</v>
+      </c>
+      <c r="I29" s="42">
+        <v>4</v>
+      </c>
+      <c r="J29" s="42">
+        <v>4</v>
+      </c>
+      <c r="K29" s="42">
+        <v>4</v>
+      </c>
+      <c r="L29" s="42">
+        <v>4</v>
+      </c>
+      <c r="M29" s="42">
+        <v>4</v>
+      </c>
+      <c r="N29" s="42">
+        <v>4</v>
+      </c>
+      <c r="O29" s="42">
+        <v>4</v>
+      </c>
+      <c r="P29" s="42">
+        <v>4</v>
+      </c>
+      <c r="Q29" s="42">
+        <v>4</v>
+      </c>
+      <c r="R29" s="42">
+        <v>4</v>
+      </c>
+      <c r="S29" s="42">
+        <v>4</v>
+      </c>
+      <c r="T29" s="42">
+        <v>4</v>
+      </c>
+      <c r="U29" s="42">
+        <v>4</v>
+      </c>
+      <c r="V29" s="42">
+        <v>4</v>
+      </c>
+      <c r="W29" s="42">
+        <v>4</v>
+      </c>
+      <c r="X29" s="42">
+        <v>4</v>
+      </c>
+      <c r="Y29" s="42">
+        <v>4</v>
+      </c>
+      <c r="Z29" s="42">
+        <v>4</v>
+      </c>
       <c r="AA29" s="6"/>
       <c r="AB29" s="7"/>
       <c r="AD29" s="12">
@@ -3029,7 +3164,7 @@
       <c r="AL29" s="34"/>
       <c r="AM29" s="5"/>
       <c r="AN29" s="18"/>
-      <c r="AO29" s="39"/>
+      <c r="AO29" s="37"/>
       <c r="AP29" s="21"/>
       <c r="AQ29" s="21"/>
       <c r="AR29" s="21"/>
@@ -3037,68 +3172,68 @@
     </row>
     <row r="30" spans="1:45" x14ac:dyDescent="0.2">
       <c r="D30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="6"/>
-      <c r="G30" s="6">
+      <c r="G30" s="61">
         <v>5</v>
       </c>
-      <c r="H30" s="6">
+      <c r="H30" s="61">
         <v>5</v>
       </c>
-      <c r="I30" s="6">
+      <c r="I30" s="61">
         <v>5</v>
       </c>
-      <c r="J30" s="6">
+      <c r="J30" s="61">
         <v>5</v>
       </c>
-      <c r="K30" s="6">
+      <c r="K30" s="61">
         <v>5</v>
       </c>
-      <c r="L30" s="6">
+      <c r="L30" s="61">
         <v>5</v>
       </c>
-      <c r="M30" s="6">
+      <c r="M30" s="61">
         <v>5</v>
       </c>
-      <c r="N30" s="6">
+      <c r="N30" s="61">
         <v>5</v>
       </c>
-      <c r="O30" s="6">
+      <c r="O30" s="61">
         <v>5</v>
       </c>
-      <c r="P30" s="6">
+      <c r="P30" s="61">
         <v>5</v>
       </c>
-      <c r="Q30" s="6">
+      <c r="Q30" s="61">
         <v>5</v>
       </c>
-      <c r="R30" s="6">
+      <c r="R30" s="61">
         <v>5</v>
       </c>
-      <c r="S30" s="6">
+      <c r="S30" s="61">
         <v>5</v>
       </c>
-      <c r="T30" s="6">
+      <c r="T30" s="61">
         <v>5</v>
       </c>
-      <c r="U30" s="6">
+      <c r="U30" s="61">
         <v>5</v>
       </c>
-      <c r="V30" s="6">
+      <c r="V30" s="61">
         <v>5</v>
       </c>
-      <c r="W30" s="6">
+      <c r="W30" s="61">
         <v>5</v>
       </c>
-      <c r="X30" s="6">
+      <c r="X30" s="61">
         <v>5</v>
       </c>
-      <c r="Y30" s="6">
+      <c r="Y30" s="61">
         <v>5</v>
       </c>
-      <c r="Z30" s="6">
+      <c r="Z30" s="61">
         <v>5</v>
       </c>
       <c r="AA30" s="6"/>
@@ -3116,7 +3251,7 @@
       <c r="AL30" s="34"/>
       <c r="AM30" s="5"/>
       <c r="AN30" s="18"/>
-      <c r="AO30" s="39"/>
+      <c r="AO30" s="37"/>
       <c r="AP30" s="21"/>
       <c r="AQ30" s="21"/>
       <c r="AR30" s="21"/>
@@ -3124,7 +3259,7 @@
     </row>
     <row r="31" spans="1:45" x14ac:dyDescent="0.2">
       <c r="D31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="6"/>
@@ -3154,40 +3289,40 @@
         <v>30</v>
       </c>
       <c r="AE31" s="19" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AF31" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AG31" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH31" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="AH31" s="19" t="s">
+      <c r="AI31" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="AJ31" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="AK31" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL31" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="AM31" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="AI31" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="AJ31" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="AK31" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="AL31" s="9" t="s">
+      <c r="AN31" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="AM31" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="AN31" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="AO31" s="40">
+      <c r="AO31" s="38">
         <v>1</v>
       </c>
       <c r="AP31" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AQ31" s="22">
         <v>10</v>
@@ -3201,7 +3336,7 @@
     </row>
     <row r="32" spans="1:45" x14ac:dyDescent="0.2">
       <c r="D32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="6"/>
@@ -3230,7 +3365,7 @@
     </row>
     <row r="33" spans="1:40" x14ac:dyDescent="0.2">
       <c r="D33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="6"/>
@@ -3257,35 +3392,35 @@
       <c r="AA33" s="6"/>
       <c r="AB33" s="7"/>
       <c r="AD33" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AE33" s="4">
         <v>10</v>
       </c>
       <c r="AF33" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AG33" s="26"/>
       <c r="AH33" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AI33" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AK33" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="AL33" s="23" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="AM33" s="33" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AN33" s="33"/>
     </row>
     <row r="34" spans="1:40" x14ac:dyDescent="0.2">
       <c r="D34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="6"/>
@@ -3312,7 +3447,7 @@
       <c r="AA34" s="6"/>
       <c r="AB34" s="7"/>
       <c r="AD34" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AE34" s="4">
         <v>10</v>
@@ -3320,20 +3455,20 @@
       <c r="AF34" s="28"/>
       <c r="AG34" s="26"/>
       <c r="AH34" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AI34" s="16">
         <v>25</v>
       </c>
       <c r="AK34" s="15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AM34" s="33"/>
       <c r="AN34" s="33"/>
     </row>
     <row r="35" spans="1:40" x14ac:dyDescent="0.2">
       <c r="D35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="6"/>
@@ -3360,7 +3495,7 @@
       <c r="AA35" s="6"/>
       <c r="AB35" s="7"/>
       <c r="AD35" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AE35" s="4">
         <v>13</v>
@@ -3368,23 +3503,23 @@
       <c r="AF35" s="28"/>
       <c r="AG35" s="26"/>
       <c r="AH35" s="27" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="AI35" s="30">
         <v>30</v>
       </c>
       <c r="AK35" s="27" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AL35" s="30" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AM35" s="33"/>
       <c r="AN35" s="33"/>
     </row>
     <row r="36" spans="1:40" x14ac:dyDescent="0.2">
       <c r="D36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="6"/>
@@ -3411,7 +3546,7 @@
       <c r="AA36" s="6"/>
       <c r="AB36" s="7"/>
       <c r="AD36" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AE36" s="4">
         <v>0</v>
@@ -3425,7 +3560,7 @@
     </row>
     <row r="37" spans="1:40" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E37" s="5"/>
       <c r="F37" s="6"/>
@@ -3452,7 +3587,7 @@
       <c r="AA37" s="6"/>
       <c r="AB37" s="7"/>
       <c r="AD37" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AE37" s="4">
         <v>0</v>
@@ -3468,7 +3603,7 @@
     </row>
     <row r="38" spans="1:40" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="6"/>
@@ -3495,7 +3630,7 @@
       <c r="AA38" s="6"/>
       <c r="AB38" s="7"/>
       <c r="AD38" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AE38" s="20">
         <v>0</v>
@@ -3503,13 +3638,13 @@
       <c r="AF38" s="28"/>
       <c r="AG38" s="26"/>
       <c r="AH38" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="AI38" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="AI38" s="16" t="s">
-        <v>91</v>
-      </c>
       <c r="AJ38" s="26" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AK38" s="24"/>
       <c r="AL38" s="25"/>
@@ -3518,7 +3653,7 @@
     </row>
     <row r="39" spans="1:40" x14ac:dyDescent="0.2">
       <c r="D39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E39" s="8"/>
       <c r="F39" s="9"/>
@@ -3545,7 +3680,7 @@
       <c r="AA39" s="9"/>
       <c r="AB39" s="10"/>
       <c r="AD39" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AE39" s="4">
         <v>10</v>
@@ -3587,7 +3722,7 @@
       <c r="AA40" s="1"/>
       <c r="AB40" s="1"/>
       <c r="AD40" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AE40" s="4">
         <v>10</v>
@@ -3598,13 +3733,13 @@
     </row>
     <row r="41" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A41" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B41" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B41" s="14" t="s">
-        <v>25</v>
-      </c>
       <c r="D41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E41">
         <v>1</v>
@@ -3679,7 +3814,7 @@
         <v>24</v>
       </c>
       <c r="AD41" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AE41" s="4">
         <v>20</v>
@@ -3690,13 +3825,13 @@
     </row>
     <row r="42" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A42" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D42" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="3"/>
@@ -3723,7 +3858,7 @@
       <c r="AA42" s="3"/>
       <c r="AB42" s="4"/>
       <c r="AD42" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AE42" s="4">
         <v>0</v>
@@ -3734,7 +3869,7 @@
     </row>
     <row r="43" spans="1:40" x14ac:dyDescent="0.2">
       <c r="D43" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E43" s="5"/>
       <c r="F43" s="6"/>
@@ -3801,7 +3936,7 @@
       <c r="AA43" s="6"/>
       <c r="AB43" s="7"/>
       <c r="AD43" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AE43" s="4">
         <v>0</v>
@@ -3812,7 +3947,7 @@
     </row>
     <row r="44" spans="1:40" x14ac:dyDescent="0.2">
       <c r="D44" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E44" s="5"/>
       <c r="F44" s="6"/>
@@ -3879,7 +4014,7 @@
       <c r="AA44" s="6"/>
       <c r="AB44" s="7"/>
       <c r="AD44" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE44" s="20">
         <v>0</v>
@@ -3889,7 +4024,7 @@
     </row>
     <row r="45" spans="1:40" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D45" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E45" s="5"/>
       <c r="F45" s="6"/>
@@ -3956,13 +4091,13 @@
       <c r="AA45" s="6"/>
       <c r="AB45" s="7"/>
       <c r="AF45" s="26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AG45" s="26"/>
     </row>
     <row r="46" spans="1:40" x14ac:dyDescent="0.2">
       <c r="D46" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E46" s="5"/>
       <c r="F46" s="6"/>
@@ -4034,7 +4169,7 @@
     </row>
     <row r="47" spans="1:40" x14ac:dyDescent="0.2">
       <c r="D47" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E47" s="5"/>
       <c r="F47" s="6"/>
@@ -4065,7 +4200,7 @@
     </row>
     <row r="48" spans="1:40" x14ac:dyDescent="0.2">
       <c r="D48" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E48" s="5"/>
       <c r="F48" s="6"/>
@@ -4096,7 +4231,7 @@
     </row>
     <row r="49" spans="1:33" x14ac:dyDescent="0.2">
       <c r="D49" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E49" s="5"/>
       <c r="F49" s="6"/>
@@ -4127,7 +4262,7 @@
     </row>
     <row r="50" spans="1:33" x14ac:dyDescent="0.2">
       <c r="D50" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E50" s="5"/>
       <c r="F50" s="6"/>
@@ -4158,7 +4293,7 @@
     </row>
     <row r="51" spans="1:33" x14ac:dyDescent="0.2">
       <c r="D51" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E51" s="5"/>
       <c r="F51" s="6"/>
@@ -4187,7 +4322,7 @@
     </row>
     <row r="52" spans="1:33" x14ac:dyDescent="0.2">
       <c r="D52" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E52" s="5"/>
       <c r="F52" s="6"/>
@@ -4216,7 +4351,7 @@
     </row>
     <row r="53" spans="1:33" x14ac:dyDescent="0.2">
       <c r="D53" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E53" s="5"/>
       <c r="F53" s="6"/>
@@ -4245,7 +4380,7 @@
     </row>
     <row r="54" spans="1:33" x14ac:dyDescent="0.2">
       <c r="D54" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E54" s="5"/>
       <c r="F54" s="6"/>
@@ -4274,7 +4409,7 @@
     </row>
     <row r="55" spans="1:33" x14ac:dyDescent="0.2">
       <c r="D55" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E55" s="5"/>
       <c r="F55" s="6"/>
@@ -4303,7 +4438,7 @@
     </row>
     <row r="56" spans="1:33" x14ac:dyDescent="0.2">
       <c r="D56" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E56" s="5"/>
       <c r="F56" s="6"/>
@@ -4332,7 +4467,7 @@
     </row>
     <row r="57" spans="1:33" x14ac:dyDescent="0.2">
       <c r="D57" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E57" s="8"/>
       <c r="F57" s="9"/>

</xml_diff>

<commit_message>
Small fixes, big effects
</commit_message>
<xml_diff>
--- a/worklist.xlsx
+++ b/worklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabewilson/Desktop/worklist_generation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/01c1829094dbd390/Desktop/Kelly_Lab/.venv/worklist_git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3241FD07-51B1-D843-BB14-40E3C738CAEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{3241FD07-51B1-D843-BB14-40E3C738CAEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C41C4AFA-ABE8-4987-BB92-FABAF33DC4B7}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="740" windowWidth="29400" windowHeight="17100" xr2:uid="{BF50EA0A-2797-EC49-8565-645DB7B38C61}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{BF50EA0A-2797-EC49-8565-645DB7B38C61}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -329,7 +329,7 @@
     <t>Doesn't use all wells in order to create blocks of the same size and evenly spaced nonsample blocks.</t>
   </si>
   <si>
-    <t>1-30</t>
+    <t>1-12</t>
   </si>
 </sst>
 </file>
@@ -559,7 +559,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
@@ -614,6 +614,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -638,17 +646,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -985,12 +982,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79332BF3-487A-D048-AE38-CBE359952258}">
   <dimension ref="A1:AS58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="40" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AD28" sqref="AD28"/>
+    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="50" zoomScaleNormal="40" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
@@ -1013,7 +1010,7 @@
     <col min="43" max="45" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.4">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1026,7 +1023,7 @@
       <c r="AE1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="AF1" s="35" t="s">
+      <c r="AF1" s="26" t="s">
         <v>4</v>
       </c>
       <c r="AG1" s="11" t="s">
@@ -1044,7 +1041,7 @@
       <c r="AK1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="AL1" s="35" t="s">
+      <c r="AL1" s="26" t="s">
         <v>10</v>
       </c>
       <c r="AM1" s="11" t="s">
@@ -1053,7 +1050,7 @@
       <c r="AN1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="AO1" s="37" t="s">
+      <c r="AO1" s="28" t="s">
         <v>60</v>
       </c>
       <c r="AP1" s="14" t="s">
@@ -1069,7 +1066,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.4">
       <c r="A2" s="15" t="s">
         <v>13</v>
       </c>
@@ -1082,7 +1079,7 @@
       <c r="AE2" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="AF2" s="36" t="s">
+      <c r="AF2" s="27" t="s">
         <v>70</v>
       </c>
       <c r="AG2" s="5" t="s">
@@ -1100,7 +1097,7 @@
       <c r="AK2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="AL2" s="34" t="s">
+      <c r="AL2" s="6" t="s">
         <v>20</v>
       </c>
       <c r="AM2" s="5" t="s">
@@ -1109,7 +1106,7 @@
       <c r="AN2" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="AO2" s="38">
+      <c r="AO2" s="29">
         <v>1</v>
       </c>
       <c r="AP2" s="21" t="s">
@@ -1119,7 +1116,7 @@
       <c r="AR2" s="21"/>
       <c r="AS2" s="21"/>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.4">
       <c r="A3" s="15" t="s">
         <v>22</v>
       </c>
@@ -1132,7 +1129,7 @@
       <c r="AE3" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="AF3" s="34" t="s">
+      <c r="AF3" s="6" t="s">
         <v>68</v>
       </c>
       <c r="AG3" s="5" t="s">
@@ -1150,7 +1147,7 @@
       <c r="AK3" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="AL3" s="34" t="s">
+      <c r="AL3" s="6" t="s">
         <v>20</v>
       </c>
       <c r="AM3" s="5" t="s">
@@ -1159,7 +1156,7 @@
       <c r="AN3" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="AO3" s="39">
+      <c r="AO3" s="30">
         <v>1</v>
       </c>
       <c r="AP3" s="21" t="s">
@@ -1175,7 +1172,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="D4" s="1"/>
@@ -1209,7 +1206,7 @@
       <c r="AE4" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="AF4" s="34" t="s">
+      <c r="AF4" s="6" t="s">
         <v>72</v>
       </c>
       <c r="AG4" s="5" t="s">
@@ -1227,7 +1224,7 @@
       <c r="AK4" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="AL4" s="34" t="s">
+      <c r="AL4" s="6" t="s">
         <v>20</v>
       </c>
       <c r="AM4" s="5" t="s">
@@ -1236,7 +1233,7 @@
       <c r="AN4" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="AO4" s="39">
+      <c r="AO4" s="30">
         <v>1</v>
       </c>
       <c r="AP4" s="21" t="s">
@@ -1252,7 +1249,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.4">
       <c r="A5" s="14" t="s">
         <v>24</v>
       </c>
@@ -1340,7 +1337,7 @@
       <c r="AE5" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="AF5" s="34" t="s">
+      <c r="AF5" s="6" t="s">
         <v>79</v>
       </c>
       <c r="AG5" s="5" t="s">
@@ -1358,7 +1355,7 @@
       <c r="AK5" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="AL5" s="34" t="s">
+      <c r="AL5" s="6" t="s">
         <v>20</v>
       </c>
       <c r="AM5" s="5" t="s">
@@ -1367,7 +1364,7 @@
       <c r="AN5" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="AO5" s="39">
+      <c r="AO5" s="30">
         <v>2</v>
       </c>
       <c r="AP5" s="21" t="s">
@@ -1377,7 +1374,7 @@
       <c r="AR5" s="21"/>
       <c r="AS5" s="21"/>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.4">
       <c r="A6" s="19" t="s">
         <v>27</v>
       </c>
@@ -1419,7 +1416,7 @@
       <c r="AE6" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="AF6" s="34" t="s">
+      <c r="AF6" s="6" t="s">
         <v>80</v>
       </c>
       <c r="AG6" s="5" t="s">
@@ -1437,7 +1434,7 @@
       <c r="AK6" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="AL6" s="34" t="s">
+      <c r="AL6" s="6" t="s">
         <v>20</v>
       </c>
       <c r="AM6" s="5" t="s">
@@ -1446,7 +1443,7 @@
       <c r="AN6" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="AO6" s="39">
+      <c r="AO6" s="30">
         <v>1</v>
       </c>
       <c r="AP6" s="21" t="s">
@@ -1456,7 +1453,7 @@
       <c r="AR6" s="21"/>
       <c r="AS6" s="21"/>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D7" t="s">
         <v>30</v>
       </c>
@@ -1488,22 +1485,22 @@
         <v>6</v>
       </c>
       <c r="AE7" s="18"/>
-      <c r="AF7" s="34"/>
+      <c r="AF7" s="6"/>
       <c r="AG7" s="5"/>
       <c r="AH7" s="18"/>
       <c r="AI7" s="7"/>
       <c r="AJ7" s="6"/>
       <c r="AK7" s="18"/>
-      <c r="AL7" s="34"/>
+      <c r="AL7" s="6"/>
       <c r="AM7" s="5"/>
       <c r="AN7" s="18"/>
-      <c r="AO7" s="39"/>
+      <c r="AO7" s="30"/>
       <c r="AP7" s="21"/>
       <c r="AQ7" s="21"/>
       <c r="AR7" s="21"/>
       <c r="AS7" s="21"/>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D8" t="s">
         <v>31</v>
       </c>
@@ -1577,7 +1574,7 @@
       <c r="AE8" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="AF8" s="34" t="s">
+      <c r="AF8" s="6" t="s">
         <v>88</v>
       </c>
       <c r="AG8" s="5" t="s">
@@ -1595,7 +1592,7 @@
       <c r="AK8" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="AL8" s="34" t="s">
+      <c r="AL8" s="6" t="s">
         <v>20</v>
       </c>
       <c r="AM8" s="5" t="s">
@@ -1604,7 +1601,7 @@
       <c r="AN8" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="AO8" s="39">
+      <c r="AO8" s="30">
         <v>1</v>
       </c>
       <c r="AP8" s="21" t="s">
@@ -1614,7 +1611,7 @@
       <c r="AR8" s="21"/>
       <c r="AS8" s="21"/>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D9" t="s">
         <v>32</v>
       </c>
@@ -1688,7 +1685,7 @@
       <c r="AE9" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="AF9" s="34" t="s">
+      <c r="AF9" s="6" t="s">
         <v>70</v>
       </c>
       <c r="AG9" s="5" t="s">
@@ -1706,7 +1703,7 @@
       <c r="AK9" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="AL9" s="34" t="s">
+      <c r="AL9" s="6" t="s">
         <v>20</v>
       </c>
       <c r="AM9" s="5" t="s">
@@ -1715,7 +1712,7 @@
       <c r="AN9" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="AO9" s="39">
+      <c r="AO9" s="30">
         <v>1</v>
       </c>
       <c r="AP9" s="21" t="s">
@@ -1725,7 +1722,7 @@
       <c r="AR9" s="21"/>
       <c r="AS9" s="21"/>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D10" t="s">
         <v>33</v>
       </c>
@@ -1799,7 +1796,7 @@
       <c r="AE10" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="AF10" s="34" t="s">
+      <c r="AF10" s="6" t="s">
         <v>81</v>
       </c>
       <c r="AG10" s="5" t="s">
@@ -1817,7 +1814,7 @@
       <c r="AK10" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="AL10" s="34" t="s">
+      <c r="AL10" s="6" t="s">
         <v>20</v>
       </c>
       <c r="AM10" s="5" t="s">
@@ -1826,7 +1823,7 @@
       <c r="AN10" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="AO10" s="39">
+      <c r="AO10" s="30">
         <v>1</v>
       </c>
       <c r="AP10" s="21" t="s">
@@ -1836,7 +1833,7 @@
       <c r="AR10" s="21"/>
       <c r="AS10" s="21"/>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D11" t="s">
         <v>34</v>
       </c>
@@ -1880,7 +1877,7 @@
       <c r="AE11" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="AF11" s="34" t="s">
+      <c r="AF11" s="6" t="s">
         <v>82</v>
       </c>
       <c r="AG11" s="5" t="s">
@@ -1898,7 +1895,7 @@
       <c r="AK11" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="AL11" s="34" t="s">
+      <c r="AL11" s="6" t="s">
         <v>20</v>
       </c>
       <c r="AM11" s="5" t="s">
@@ -1907,7 +1904,7 @@
       <c r="AN11" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="AO11" s="39">
+      <c r="AO11" s="30">
         <v>1</v>
       </c>
       <c r="AP11" s="21" t="s">
@@ -1917,7 +1914,7 @@
       <c r="AR11" s="21"/>
       <c r="AS11" s="21"/>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D12" t="s">
         <v>35</v>
       </c>
@@ -1991,7 +1988,7 @@
       <c r="AE12" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="AF12" s="34" t="s">
+      <c r="AF12" s="6" t="s">
         <v>87</v>
       </c>
       <c r="AG12" s="5" t="s">
@@ -2009,7 +2006,7 @@
       <c r="AK12" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="AL12" s="34" t="s">
+      <c r="AL12" s="6" t="s">
         <v>20</v>
       </c>
       <c r="AM12" s="5" t="s">
@@ -2018,7 +2015,7 @@
       <c r="AN12" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="AO12" s="39">
+      <c r="AO12" s="30">
         <v>1</v>
       </c>
       <c r="AP12" s="21" t="s">
@@ -2028,7 +2025,7 @@
       <c r="AR12" s="21"/>
       <c r="AS12" s="21"/>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D13" t="s">
         <v>36</v>
       </c>
@@ -2062,7 +2059,7 @@
       <c r="AE13" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="AF13" s="34" t="s">
+      <c r="AF13" s="6" t="s">
         <v>92</v>
       </c>
       <c r="AG13" s="5" t="s">
@@ -2080,7 +2077,7 @@
       <c r="AK13" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="AL13" s="34" t="s">
+      <c r="AL13" s="6" t="s">
         <v>20</v>
       </c>
       <c r="AM13" s="5" t="s">
@@ -2089,7 +2086,7 @@
       <c r="AN13" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="AO13" s="39">
+      <c r="AO13" s="30">
         <v>1</v>
       </c>
       <c r="AP13" s="21" t="s">
@@ -2099,7 +2096,7 @@
       <c r="AR13" s="21"/>
       <c r="AS13" s="21"/>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D14" t="s">
         <v>37</v>
       </c>
@@ -2131,22 +2128,22 @@
         <v>13</v>
       </c>
       <c r="AE14" s="18"/>
-      <c r="AF14" s="34"/>
+      <c r="AF14" s="6"/>
       <c r="AG14" s="5"/>
       <c r="AH14" s="18"/>
       <c r="AI14" s="7"/>
       <c r="AJ14" s="6"/>
       <c r="AK14" s="18"/>
-      <c r="AL14" s="34"/>
+      <c r="AL14" s="6"/>
       <c r="AM14" s="5"/>
       <c r="AN14" s="18"/>
-      <c r="AO14" s="39"/>
+      <c r="AO14" s="30"/>
       <c r="AP14" s="21"/>
       <c r="AQ14" s="21"/>
       <c r="AR14" s="21"/>
       <c r="AS14" s="21"/>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D15" t="s">
         <v>38</v>
       </c>
@@ -2178,22 +2175,22 @@
         <v>14</v>
       </c>
       <c r="AE15" s="18"/>
-      <c r="AF15" s="34"/>
+      <c r="AF15" s="6"/>
       <c r="AG15" s="5"/>
       <c r="AH15" s="18"/>
       <c r="AI15" s="7"/>
       <c r="AJ15" s="6"/>
       <c r="AK15" s="18"/>
-      <c r="AL15" s="34"/>
+      <c r="AL15" s="6"/>
       <c r="AM15" s="5"/>
       <c r="AN15" s="18"/>
-      <c r="AO15" s="39"/>
+      <c r="AO15" s="30"/>
       <c r="AP15" s="21"/>
       <c r="AQ15" s="21"/>
       <c r="AR15" s="21"/>
       <c r="AS15" s="21"/>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D16" t="s">
         <v>39</v>
       </c>
@@ -2229,22 +2226,22 @@
         <v>15</v>
       </c>
       <c r="AE16" s="18"/>
-      <c r="AF16" s="34"/>
+      <c r="AF16" s="6"/>
       <c r="AG16" s="5"/>
       <c r="AH16" s="18"/>
       <c r="AI16" s="7"/>
       <c r="AJ16" s="6"/>
       <c r="AK16" s="18"/>
-      <c r="AL16" s="34"/>
+      <c r="AL16" s="6"/>
       <c r="AM16" s="5"/>
       <c r="AN16" s="18"/>
-      <c r="AO16" s="39"/>
+      <c r="AO16" s="30"/>
       <c r="AP16" s="21"/>
       <c r="AQ16" s="21"/>
       <c r="AR16" s="21"/>
       <c r="AS16" s="21"/>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D17" t="s">
         <v>40</v>
       </c>
@@ -2276,22 +2273,22 @@
         <v>16</v>
       </c>
       <c r="AE17" s="18"/>
-      <c r="AF17" s="34"/>
+      <c r="AF17" s="6"/>
       <c r="AG17" s="5"/>
       <c r="AH17" s="18"/>
       <c r="AI17" s="7"/>
       <c r="AJ17" s="6"/>
       <c r="AK17" s="18"/>
-      <c r="AL17" s="34"/>
+      <c r="AL17" s="6"/>
       <c r="AM17" s="5"/>
       <c r="AN17" s="18"/>
-      <c r="AO17" s="39"/>
+      <c r="AO17" s="30"/>
       <c r="AP17" s="21"/>
       <c r="AQ17" s="21"/>
       <c r="AR17" s="21"/>
       <c r="AS17" s="21"/>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D18" t="s">
         <v>41</v>
       </c>
@@ -2323,22 +2320,22 @@
         <v>17</v>
       </c>
       <c r="AE18" s="18"/>
-      <c r="AF18" s="34"/>
+      <c r="AF18" s="6"/>
       <c r="AG18" s="5"/>
       <c r="AH18" s="18"/>
       <c r="AI18" s="7"/>
       <c r="AJ18" s="6"/>
       <c r="AK18" s="18"/>
-      <c r="AL18" s="34"/>
+      <c r="AL18" s="6"/>
       <c r="AM18" s="5"/>
       <c r="AN18" s="18"/>
-      <c r="AO18" s="39"/>
+      <c r="AO18" s="30"/>
       <c r="AP18" s="21"/>
       <c r="AQ18" s="21"/>
       <c r="AR18" s="21"/>
       <c r="AS18" s="21"/>
     </row>
-    <row r="19" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D19" t="s">
         <v>42</v>
       </c>
@@ -2370,22 +2367,22 @@
         <v>18</v>
       </c>
       <c r="AE19" s="18"/>
-      <c r="AF19" s="34"/>
+      <c r="AF19" s="6"/>
       <c r="AG19" s="5"/>
       <c r="AH19" s="18"/>
       <c r="AI19" s="7"/>
       <c r="AJ19" s="6"/>
       <c r="AK19" s="18"/>
-      <c r="AL19" s="34"/>
+      <c r="AL19" s="6"/>
       <c r="AM19" s="5"/>
       <c r="AN19" s="18"/>
-      <c r="AO19" s="39"/>
+      <c r="AO19" s="30"/>
       <c r="AP19" s="21"/>
       <c r="AQ19" s="21"/>
       <c r="AR19" s="21"/>
       <c r="AS19" s="21"/>
     </row>
-    <row r="20" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D20" t="s">
         <v>43</v>
       </c>
@@ -2417,22 +2414,22 @@
         <v>19</v>
       </c>
       <c r="AE20" s="18"/>
-      <c r="AF20" s="34"/>
+      <c r="AF20" s="6"/>
       <c r="AG20" s="5"/>
       <c r="AH20" s="18"/>
       <c r="AI20" s="7"/>
       <c r="AJ20" s="6"/>
       <c r="AK20" s="18"/>
-      <c r="AL20" s="34"/>
+      <c r="AL20" s="6"/>
       <c r="AM20" s="5"/>
       <c r="AN20" s="18"/>
-      <c r="AO20" s="39"/>
+      <c r="AO20" s="30"/>
       <c r="AP20" s="21"/>
       <c r="AQ20" s="21"/>
       <c r="AR20" s="21"/>
       <c r="AS20" s="21"/>
     </row>
-    <row r="21" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D21" t="s">
         <v>44</v>
       </c>
@@ -2464,22 +2461,22 @@
         <v>20</v>
       </c>
       <c r="AE21" s="18"/>
-      <c r="AF21" s="34"/>
+      <c r="AF21" s="6"/>
       <c r="AG21" s="5"/>
       <c r="AH21" s="18"/>
       <c r="AI21" s="7"/>
       <c r="AJ21" s="6"/>
       <c r="AK21" s="18"/>
-      <c r="AL21" s="34"/>
+      <c r="AL21" s="6"/>
       <c r="AM21" s="5"/>
       <c r="AN21" s="18"/>
-      <c r="AO21" s="39"/>
+      <c r="AO21" s="30"/>
       <c r="AP21" s="21"/>
       <c r="AQ21" s="21"/>
       <c r="AR21" s="21"/>
       <c r="AS21" s="21"/>
     </row>
-    <row r="22" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:45" x14ac:dyDescent="0.4">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="D22" s="1"/>
@@ -2511,22 +2508,22 @@
         <v>21</v>
       </c>
       <c r="AE22" s="18"/>
-      <c r="AF22" s="34"/>
+      <c r="AF22" s="6"/>
       <c r="AG22" s="5"/>
       <c r="AH22" s="18"/>
       <c r="AI22" s="7"/>
       <c r="AJ22" s="6"/>
       <c r="AK22" s="18"/>
-      <c r="AL22" s="34"/>
+      <c r="AL22" s="6"/>
       <c r="AM22" s="5"/>
       <c r="AN22" s="18"/>
-      <c r="AO22" s="39"/>
+      <c r="AO22" s="30"/>
       <c r="AP22" s="21"/>
       <c r="AQ22" s="21"/>
       <c r="AR22" s="21"/>
       <c r="AS22" s="21"/>
     </row>
-    <row r="23" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:45" x14ac:dyDescent="0.4">
       <c r="A23" s="14" t="s">
         <v>24</v>
       </c>
@@ -2612,22 +2609,22 @@
         <v>22</v>
       </c>
       <c r="AE23" s="18"/>
-      <c r="AF23" s="34"/>
+      <c r="AF23" s="6"/>
       <c r="AG23" s="5"/>
       <c r="AH23" s="18"/>
       <c r="AI23" s="7"/>
       <c r="AJ23" s="6"/>
       <c r="AK23" s="18"/>
-      <c r="AL23" s="34"/>
+      <c r="AL23" s="6"/>
       <c r="AM23" s="5"/>
       <c r="AN23" s="18"/>
-      <c r="AO23" s="39"/>
+      <c r="AO23" s="30"/>
       <c r="AP23" s="21"/>
       <c r="AQ23" s="21"/>
       <c r="AR23" s="21"/>
       <c r="AS23" s="21"/>
     </row>
-    <row r="24" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:45" x14ac:dyDescent="0.4">
       <c r="A24" s="19" t="s">
         <v>30</v>
       </c>
@@ -2665,22 +2662,22 @@
         <v>23</v>
       </c>
       <c r="AE24" s="18"/>
-      <c r="AF24" s="34"/>
+      <c r="AF24" s="6"/>
       <c r="AG24" s="5"/>
       <c r="AH24" s="18"/>
       <c r="AI24" s="7"/>
       <c r="AJ24" s="6"/>
       <c r="AK24" s="18"/>
-      <c r="AL24" s="34"/>
+      <c r="AL24" s="6"/>
       <c r="AM24" s="5"/>
       <c r="AN24" s="18"/>
-      <c r="AO24" s="39"/>
+      <c r="AO24" s="30"/>
       <c r="AP24" s="21"/>
       <c r="AQ24" s="21"/>
       <c r="AR24" s="21"/>
       <c r="AS24" s="21"/>
     </row>
-    <row r="25" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D25" t="s">
         <v>30</v>
       </c>
@@ -2712,22 +2709,22 @@
         <v>24</v>
       </c>
       <c r="AE25" s="18"/>
-      <c r="AF25" s="34"/>
+      <c r="AF25" s="6"/>
       <c r="AG25" s="5"/>
       <c r="AH25" s="18"/>
       <c r="AI25" s="7"/>
       <c r="AJ25" s="6"/>
       <c r="AK25" s="18"/>
-      <c r="AL25" s="34"/>
+      <c r="AL25" s="6"/>
       <c r="AM25" s="5"/>
       <c r="AN25" s="18"/>
-      <c r="AO25" s="39"/>
+      <c r="AO25" s="30"/>
       <c r="AP25" s="21"/>
       <c r="AQ25" s="21"/>
       <c r="AR25" s="21"/>
       <c r="AS25" s="21"/>
     </row>
-    <row r="26" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D26" t="s">
         <v>31</v>
       </c>
@@ -2799,22 +2796,22 @@
         <v>25</v>
       </c>
       <c r="AE26" s="18"/>
-      <c r="AF26" s="34"/>
+      <c r="AF26" s="6"/>
       <c r="AG26" s="5"/>
       <c r="AH26" s="18"/>
       <c r="AI26" s="7"/>
       <c r="AJ26" s="6"/>
       <c r="AK26" s="18"/>
-      <c r="AL26" s="34"/>
+      <c r="AL26" s="6"/>
       <c r="AM26" s="5"/>
       <c r="AN26" s="18"/>
-      <c r="AO26" s="39"/>
+      <c r="AO26" s="30"/>
       <c r="AP26" s="21"/>
       <c r="AQ26" s="21"/>
       <c r="AR26" s="21"/>
       <c r="AS26" s="21"/>
     </row>
-    <row r="27" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D27" t="s">
         <v>32</v>
       </c>
@@ -2886,22 +2883,22 @@
         <v>26</v>
       </c>
       <c r="AE27" s="18"/>
-      <c r="AF27" s="34"/>
+      <c r="AF27" s="6"/>
       <c r="AG27" s="5"/>
       <c r="AH27" s="18"/>
       <c r="AI27" s="7"/>
       <c r="AJ27" s="6"/>
       <c r="AK27" s="18"/>
-      <c r="AL27" s="34"/>
+      <c r="AL27" s="6"/>
       <c r="AM27" s="5"/>
       <c r="AN27" s="18"/>
-      <c r="AO27" s="39"/>
+      <c r="AO27" s="30"/>
       <c r="AP27" s="21"/>
       <c r="AQ27" s="21"/>
       <c r="AR27" s="21"/>
       <c r="AS27" s="21"/>
     </row>
-    <row r="28" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D28" t="s">
         <v>33</v>
       </c>
@@ -2973,22 +2970,22 @@
         <v>27</v>
       </c>
       <c r="AE28" s="18"/>
-      <c r="AF28" s="34"/>
+      <c r="AF28" s="6"/>
       <c r="AG28" s="5"/>
       <c r="AH28" s="18"/>
       <c r="AI28" s="7"/>
       <c r="AJ28" s="6"/>
       <c r="AK28" s="18"/>
-      <c r="AL28" s="34"/>
+      <c r="AL28" s="6"/>
       <c r="AM28" s="5"/>
       <c r="AN28" s="18"/>
-      <c r="AO28" s="39"/>
+      <c r="AO28" s="30"/>
       <c r="AP28" s="21"/>
       <c r="AQ28" s="21"/>
       <c r="AR28" s="21"/>
       <c r="AS28" s="21"/>
     </row>
-    <row r="29" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D29" t="s">
         <v>34</v>
       </c>
@@ -3020,22 +3017,22 @@
         <v>28</v>
       </c>
       <c r="AE29" s="18"/>
-      <c r="AF29" s="34"/>
+      <c r="AF29" s="6"/>
       <c r="AG29" s="5"/>
       <c r="AH29" s="18"/>
       <c r="AI29" s="7"/>
       <c r="AJ29" s="6"/>
       <c r="AK29" s="18"/>
-      <c r="AL29" s="34"/>
+      <c r="AL29" s="6"/>
       <c r="AM29" s="5"/>
       <c r="AN29" s="18"/>
-      <c r="AO29" s="39"/>
+      <c r="AO29" s="30"/>
       <c r="AP29" s="21"/>
       <c r="AQ29" s="21"/>
       <c r="AR29" s="21"/>
       <c r="AS29" s="21"/>
     </row>
-    <row r="30" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D30" t="s">
         <v>35</v>
       </c>
@@ -3107,22 +3104,22 @@
         <v>29</v>
       </c>
       <c r="AE30" s="18"/>
-      <c r="AF30" s="34"/>
+      <c r="AF30" s="6"/>
       <c r="AG30" s="5"/>
       <c r="AH30" s="18"/>
       <c r="AI30" s="7"/>
       <c r="AJ30" s="6"/>
       <c r="AK30" s="18"/>
-      <c r="AL30" s="34"/>
+      <c r="AL30" s="6"/>
       <c r="AM30" s="5"/>
       <c r="AN30" s="18"/>
-      <c r="AO30" s="39"/>
+      <c r="AO30" s="30"/>
       <c r="AP30" s="21"/>
       <c r="AQ30" s="21"/>
       <c r="AR30" s="21"/>
       <c r="AS30" s="21"/>
     </row>
-    <row r="31" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D31" t="s">
         <v>36</v>
       </c>
@@ -3183,7 +3180,7 @@
       <c r="AN31" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="AO31" s="40">
+      <c r="AO31" s="31">
         <v>1</v>
       </c>
       <c r="AP31" s="22" t="s">
@@ -3199,7 +3196,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:45" x14ac:dyDescent="0.4">
       <c r="D32" t="s">
         <v>37</v>
       </c>
@@ -3228,7 +3225,7 @@
       <c r="AA32" s="6"/>
       <c r="AB32" s="7"/>
     </row>
-    <row r="33" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:40" x14ac:dyDescent="0.4">
       <c r="D33" t="s">
         <v>38</v>
       </c>
@@ -3262,10 +3259,10 @@
       <c r="AE33" s="4">
         <v>10</v>
       </c>
-      <c r="AF33" s="28" t="s">
+      <c r="AF33" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="AG33" s="26"/>
+      <c r="AG33" s="32"/>
       <c r="AH33" s="15" t="s">
         <v>64</v>
       </c>
@@ -3278,12 +3275,12 @@
       <c r="AL33" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="AM33" s="33" t="s">
+      <c r="AM33" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="AN33" s="33"/>
-    </row>
-    <row r="34" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AN33" s="39"/>
+    </row>
+    <row r="34" spans="1:40" x14ac:dyDescent="0.4">
       <c r="D34" t="s">
         <v>39</v>
       </c>
@@ -3317,8 +3314,8 @@
       <c r="AE34" s="4">
         <v>10</v>
       </c>
-      <c r="AF34" s="28"/>
-      <c r="AG34" s="26"/>
+      <c r="AF34" s="34"/>
+      <c r="AG34" s="32"/>
       <c r="AH34" s="15" t="s">
         <v>65</v>
       </c>
@@ -3328,10 +3325,10 @@
       <c r="AK34" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="AM34" s="33"/>
-      <c r="AN34" s="33"/>
-    </row>
-    <row r="35" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AM34" s="39"/>
+      <c r="AN34" s="39"/>
+    </row>
+    <row r="35" spans="1:40" x14ac:dyDescent="0.4">
       <c r="D35" t="s">
         <v>40</v>
       </c>
@@ -3365,24 +3362,24 @@
       <c r="AE35" s="4">
         <v>13</v>
       </c>
-      <c r="AF35" s="28"/>
-      <c r="AG35" s="26"/>
-      <c r="AH35" s="27" t="s">
+      <c r="AF35" s="34"/>
+      <c r="AG35" s="32"/>
+      <c r="AH35" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="AI35" s="30">
+      <c r="AI35" s="36">
         <v>30</v>
       </c>
-      <c r="AK35" s="27" t="s">
+      <c r="AK35" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="AL35" s="30" t="s">
+      <c r="AL35" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="AM35" s="33"/>
-      <c r="AN35" s="33"/>
-    </row>
-    <row r="36" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AM35" s="39"/>
+      <c r="AN35" s="39"/>
+    </row>
+    <row r="36" spans="1:40" x14ac:dyDescent="0.4">
       <c r="D36" t="s">
         <v>41</v>
       </c>
@@ -3416,14 +3413,14 @@
       <c r="AE36" s="4">
         <v>0</v>
       </c>
-      <c r="AF36" s="28"/>
-      <c r="AG36" s="26"/>
-      <c r="AH36" s="28"/>
-      <c r="AI36" s="31"/>
-      <c r="AK36" s="29"/>
-      <c r="AL36" s="32"/>
-    </row>
-    <row r="37" spans="1:40" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF36" s="34"/>
+      <c r="AG36" s="32"/>
+      <c r="AH36" s="34"/>
+      <c r="AI36" s="37"/>
+      <c r="AK36" s="35"/>
+      <c r="AL36" s="38"/>
+    </row>
+    <row r="37" spans="1:40" ht="16" customHeight="1" x14ac:dyDescent="0.4">
       <c r="D37" t="s">
         <v>42</v>
       </c>
@@ -3457,16 +3454,16 @@
       <c r="AE37" s="4">
         <v>0</v>
       </c>
-      <c r="AF37" s="28"/>
-      <c r="AG37" s="26"/>
-      <c r="AH37" s="29"/>
-      <c r="AI37" s="32"/>
+      <c r="AF37" s="34"/>
+      <c r="AG37" s="32"/>
+      <c r="AH37" s="35"/>
+      <c r="AI37" s="38"/>
       <c r="AK37" s="24"/>
       <c r="AL37" s="25"/>
       <c r="AM37" s="24"/>
       <c r="AN37" s="24"/>
     </row>
-    <row r="38" spans="1:40" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:40" ht="16" customHeight="1" x14ac:dyDescent="0.4">
       <c r="D38" t="s">
         <v>43</v>
       </c>
@@ -3500,15 +3497,15 @@
       <c r="AE38" s="20">
         <v>0</v>
       </c>
-      <c r="AF38" s="28"/>
-      <c r="AG38" s="26"/>
+      <c r="AF38" s="34"/>
+      <c r="AG38" s="32"/>
       <c r="AH38" s="15" t="s">
         <v>89</v>
       </c>
       <c r="AI38" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="AJ38" s="26" t="s">
+      <c r="AJ38" s="32" t="s">
         <v>96</v>
       </c>
       <c r="AK38" s="24"/>
@@ -3516,7 +3513,7 @@
       <c r="AM38" s="24"/>
       <c r="AN38" s="24"/>
     </row>
-    <row r="39" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:40" x14ac:dyDescent="0.4">
       <c r="D39" t="s">
         <v>44</v>
       </c>
@@ -3550,15 +3547,15 @@
       <c r="AE39" s="4">
         <v>10</v>
       </c>
-      <c r="AF39" s="28"/>
-      <c r="AG39" s="26"/>
-      <c r="AJ39" s="26"/>
+      <c r="AF39" s="34"/>
+      <c r="AG39" s="32"/>
+      <c r="AJ39" s="32"/>
       <c r="AK39" s="24"/>
       <c r="AL39" s="25"/>
       <c r="AM39" s="24"/>
       <c r="AN39" s="24"/>
     </row>
-    <row r="40" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:40" x14ac:dyDescent="0.4">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="D40" s="1"/>
@@ -3592,11 +3589,11 @@
       <c r="AE40" s="4">
         <v>10</v>
       </c>
-      <c r="AF40" s="28"/>
-      <c r="AG40" s="26"/>
-      <c r="AJ40" s="26"/>
-    </row>
-    <row r="41" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AF40" s="34"/>
+      <c r="AG40" s="32"/>
+      <c r="AJ40" s="32"/>
+    </row>
+    <row r="41" spans="1:40" x14ac:dyDescent="0.4">
       <c r="A41" s="14" t="s">
         <v>24</v>
       </c>
@@ -3684,11 +3681,11 @@
       <c r="AE41" s="4">
         <v>20</v>
       </c>
-      <c r="AF41" s="28"/>
-      <c r="AG41" s="26"/>
-      <c r="AJ41" s="26"/>
-    </row>
-    <row r="42" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AF41" s="34"/>
+      <c r="AG41" s="32"/>
+      <c r="AJ41" s="32"/>
+    </row>
+    <row r="42" spans="1:40" x14ac:dyDescent="0.4">
       <c r="A42" s="19" t="s">
         <v>35</v>
       </c>
@@ -3728,11 +3725,11 @@
       <c r="AE42" s="4">
         <v>0</v>
       </c>
-      <c r="AF42" s="28"/>
-      <c r="AG42" s="26"/>
-      <c r="AJ42" s="26"/>
-    </row>
-    <row r="43" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AF42" s="34"/>
+      <c r="AG42" s="32"/>
+      <c r="AJ42" s="32"/>
+    </row>
+    <row r="43" spans="1:40" x14ac:dyDescent="0.4">
       <c r="D43" t="s">
         <v>30</v>
       </c>
@@ -3806,11 +3803,11 @@
       <c r="AE43" s="4">
         <v>0</v>
       </c>
-      <c r="AF43" s="28"/>
-      <c r="AG43" s="26"/>
-      <c r="AJ43" s="26"/>
-    </row>
-    <row r="44" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AF43" s="34"/>
+      <c r="AG43" s="32"/>
+      <c r="AJ43" s="32"/>
+    </row>
+    <row r="44" spans="1:40" x14ac:dyDescent="0.4">
       <c r="D44" t="s">
         <v>31</v>
       </c>
@@ -3884,10 +3881,10 @@
       <c r="AE44" s="20">
         <v>0</v>
       </c>
-      <c r="AF44" s="28"/>
-      <c r="AG44" s="26"/>
-    </row>
-    <row r="45" spans="1:40" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF44" s="34"/>
+      <c r="AG44" s="32"/>
+    </row>
+    <row r="45" spans="1:40" ht="16" customHeight="1" x14ac:dyDescent="0.4">
       <c r="D45" t="s">
         <v>32</v>
       </c>
@@ -3955,12 +3952,12 @@
       </c>
       <c r="AA45" s="6"/>
       <c r="AB45" s="7"/>
-      <c r="AF45" s="26" t="s">
+      <c r="AF45" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="AG45" s="26"/>
-    </row>
-    <row r="46" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AG45" s="32"/>
+    </row>
+    <row r="46" spans="1:40" x14ac:dyDescent="0.4">
       <c r="D46" t="s">
         <v>33</v>
       </c>
@@ -4029,10 +4026,10 @@
       <c r="AA46" s="6"/>
       <c r="AB46" s="7"/>
       <c r="AE46" s="6"/>
-      <c r="AF46" s="26"/>
-      <c r="AG46" s="26"/>
-    </row>
-    <row r="47" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AF46" s="32"/>
+      <c r="AG46" s="32"/>
+    </row>
+    <row r="47" spans="1:40" x14ac:dyDescent="0.4">
       <c r="D47" t="s">
         <v>34</v>
       </c>
@@ -4060,10 +4057,10 @@
       <c r="Z47" s="6"/>
       <c r="AA47" s="6"/>
       <c r="AB47" s="7"/>
-      <c r="AF47" s="26"/>
-      <c r="AG47" s="26"/>
-    </row>
-    <row r="48" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AF47" s="32"/>
+      <c r="AG47" s="32"/>
+    </row>
+    <row r="48" spans="1:40" x14ac:dyDescent="0.4">
       <c r="D48" t="s">
         <v>35</v>
       </c>
@@ -4094,7 +4091,7 @@
       <c r="AF48" s="24"/>
       <c r="AG48" s="24"/>
     </row>
-    <row r="49" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:33" x14ac:dyDescent="0.4">
       <c r="D49" t="s">
         <v>36</v>
       </c>
@@ -4125,7 +4122,7 @@
       <c r="AF49" s="24"/>
       <c r="AG49" s="24"/>
     </row>
-    <row r="50" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:33" x14ac:dyDescent="0.4">
       <c r="D50" t="s">
         <v>37</v>
       </c>
@@ -4156,7 +4153,7 @@
       <c r="AF50" s="24"/>
       <c r="AG50" s="24"/>
     </row>
-    <row r="51" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:33" x14ac:dyDescent="0.4">
       <c r="D51" t="s">
         <v>38</v>
       </c>
@@ -4185,7 +4182,7 @@
       <c r="AA51" s="6"/>
       <c r="AB51" s="7"/>
     </row>
-    <row r="52" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:33" x14ac:dyDescent="0.4">
       <c r="D52" t="s">
         <v>39</v>
       </c>
@@ -4214,7 +4211,7 @@
       <c r="AA52" s="6"/>
       <c r="AB52" s="7"/>
     </row>
-    <row r="53" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:33" x14ac:dyDescent="0.4">
       <c r="D53" t="s">
         <v>40</v>
       </c>
@@ -4243,7 +4240,7 @@
       <c r="AA53" s="6"/>
       <c r="AB53" s="7"/>
     </row>
-    <row r="54" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:33" x14ac:dyDescent="0.4">
       <c r="D54" t="s">
         <v>41</v>
       </c>
@@ -4272,7 +4269,7 @@
       <c r="AA54" s="6"/>
       <c r="AB54" s="7"/>
     </row>
-    <row r="55" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:33" x14ac:dyDescent="0.4">
       <c r="D55" t="s">
         <v>42</v>
       </c>
@@ -4301,7 +4298,7 @@
       <c r="AA55" s="6"/>
       <c r="AB55" s="7"/>
     </row>
-    <row r="56" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:33" x14ac:dyDescent="0.4">
       <c r="D56" t="s">
         <v>43</v>
       </c>
@@ -4330,7 +4327,7 @@
       <c r="AA56" s="6"/>
       <c r="AB56" s="7"/>
     </row>
-    <row r="57" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:33" x14ac:dyDescent="0.4">
       <c r="D57" t="s">
         <v>44</v>
       </c>
@@ -4359,7 +4356,7 @@
       <c r="AA57" s="9"/>
       <c r="AB57" s="10"/>
     </row>
-    <row r="58" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="D58" s="1"/>

</xml_diff>